<commit_message>
Some work on preparing data
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>SVM</t>
   </si>
@@ -51,13 +51,28 @@
   </si>
   <si>
     <t>Columbia</t>
+  </si>
+  <si>
+    <t>Eyes (nopose)</t>
+  </si>
+  <si>
+    <t>Eyes (withpose)</t>
+  </si>
+  <si>
+    <t>Optimization complete. Best validation score of 3.000000 % obtained at iteration 28923, with test performance 6.000000 %</t>
+  </si>
+  <si>
+    <t>Eyes easier nopose</t>
+  </si>
+  <si>
+    <t>Eyes easier withpose</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,6 +87,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -94,11 +115,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -379,15 +408,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -431,6 +461,38 @@
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="5">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Work on MLP, Hinton plot, etc.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12225" windowHeight="10080"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="12225" windowHeight="10080"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,55 +24,46 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <si>
-    <t>SVM</t>
-  </si>
-  <si>
-    <t>RF</t>
-  </si>
-  <si>
-    <t>MLP</t>
-  </si>
-  <si>
-    <t>CNN</t>
-  </si>
-  <si>
-    <t>Pixels</t>
-  </si>
-  <si>
-    <t>PCs</t>
-  </si>
-  <si>
-    <t>HOG</t>
-  </si>
-  <si>
-    <t>LBP</t>
-  </si>
-  <si>
-    <t>Columbia</t>
-  </si>
-  <si>
-    <t>Eyes (nopose)</t>
-  </si>
-  <si>
-    <t>Eyes (withpose)</t>
-  </si>
-  <si>
-    <t>Optimization complete. Best validation score of 3.000000 % obtained at iteration 28923, with test performance 6.000000 %</t>
-  </si>
-  <si>
-    <t>Eyes easier nopose</t>
-  </si>
-  <si>
-    <t>Eyes easier withpose</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t>Dataset</t>
+  </si>
+  <si>
+    <t>eyes_withpose_PCs</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t>PCA for 90% of variance, includes head pose as Euler angles, MLP (200 hidden)</t>
+  </si>
+  <si>
+    <t>Validation</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>eyes_nopose_PCs</t>
+  </si>
+  <si>
+    <t>PCA for 90% of variance, no head pose, MLP (100 hidden)</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Not much difference between these two. Not sure adding head-pose as Euler angles helps.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,6 +83,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
       <family val="3"/>
     </font>
   </fonts>
@@ -115,11 +112,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -128,6 +122,15 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,96 +411,94 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="80.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
+        <v>41939</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0.02</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>41940</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="2">
-        <v>0.22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="4">
-        <v>0.17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="5">
+      <c r="D3" s="1">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="E3" s="4">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="F3" s="9"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="3"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>